<commit_message>
Avance muestreo de datos SpaOnline
</commit_message>
<xml_diff>
--- a/SpaOnline/CitaReserva - Muestreo Datos.xlsx
+++ b/SpaOnline/CitaReserva - Muestreo Datos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DOO\DOO\SpaOnline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DCBC24-11BF-494D-96D6-C949AE2F59A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9350FCD-CEE9-4D09-96E5-9C4E3FD6F55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="1" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -74,18 +74,12 @@
     <t>Contextro</t>
   </si>
   <si>
-    <t>Fabricante</t>
-  </si>
-  <si>
     <t>Propio</t>
   </si>
   <si>
     <t>Identificador</t>
   </si>
   <si>
-    <t>Nombre</t>
-  </si>
-  <si>
     <t>Combinacion única</t>
   </si>
   <si>
@@ -98,9 +92,6 @@
     <t>Sucursales</t>
   </si>
   <si>
-    <t>Objeto de dominio que contiene la informacion de las sucursales del Spa</t>
-  </si>
-  <si>
     <t>Servicio</t>
   </si>
   <si>
@@ -108,13 +99,121 @@
   </si>
   <si>
     <t>Objeto de dominio que contiene la informacion de las reservas de las citas del Spa</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene la informacion de la ubicación de las sucursales del Spa</t>
+  </si>
+  <si>
+    <t>Referenciado</t>
+  </si>
+  <si>
+    <t>País</t>
+  </si>
+  <si>
+    <t>Departamento</t>
+  </si>
+  <si>
+    <t>Ciudad</t>
+  </si>
+  <si>
+    <t>Sucursal</t>
+  </si>
+  <si>
+    <t>Ubicación</t>
+  </si>
+  <si>
+    <t>Combinación única</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>Antioquia</t>
+  </si>
+  <si>
+    <t>Medellín</t>
+  </si>
+  <si>
+    <t>El poblado</t>
+  </si>
+  <si>
+    <t>CL 10 43 A 29</t>
+  </si>
+  <si>
+    <t>Cundinamarca</t>
+  </si>
+  <si>
+    <t>Bogotá</t>
+  </si>
+  <si>
+    <t>Chapinero</t>
+  </si>
+  <si>
+    <t>CL 63 9 36</t>
+  </si>
+  <si>
+    <t>Atlántico</t>
+  </si>
+  <si>
+    <t>Cartagena</t>
+  </si>
+  <si>
+    <t>Bocagrande</t>
+  </si>
+  <si>
+    <t>CR 2 5 39</t>
+  </si>
+  <si>
+    <t>Limpieza facial</t>
+  </si>
+  <si>
+    <t>Masaje completo</t>
+  </si>
+  <si>
+    <t>Chocolaterapia</t>
+  </si>
+  <si>
+    <t>Nombre Servicio</t>
+  </si>
+  <si>
+    <t>Estado de la reserva</t>
+  </si>
+  <si>
+    <t>Reservado</t>
+  </si>
+  <si>
+    <t>No Reservado</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t>3:00pm</t>
+  </si>
+  <si>
+    <t>10:00am</t>
+  </si>
+  <si>
+    <t>12:30pm</t>
+  </si>
+  <si>
+    <t>16/03/2024</t>
+  </si>
+  <si>
+    <t>28/04/2024</t>
+  </si>
+  <si>
+    <t>05/05/2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,6 +225,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,10 +282,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -197,8 +305,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -616,8 +733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -644,113 +761,170 @@
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>5</v>
-      </c>
       <c r="D4" s="8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1" xr:uid="{8EFF29E0-6B07-4522-918B-B10FC37D7D6D}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{D85578A5-01DB-4CE4-84EB-E6E7CC86B3E6}"/>
+    <hyperlink ref="C3" location="Sucursales!A1" display="Referenciado" xr:uid="{C2C27A26-9F26-4F3C-9EC9-DC99886623EE}"/>
+    <hyperlink ref="C4" location="Servicios!A1" display="Referenciado" xr:uid="{B7D4804B-6051-4D79-AD41-2B1639254A0D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="58.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="5" t="str">
-        <f>B2&amp;"-"&amp;C2</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B2" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="5" t="str">
+        <f>+B2&amp;"-"&amp;C2&amp;"-"&amp;D2&amp;"-"&amp;E2&amp;"-"&amp;F2</f>
+        <v>16/03/2024-3:00pm-Reservado-Limpieza facial-El poblado</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="5" t="str">
-        <f t="shared" ref="D3:D4" si="0">B3&amp;"-"&amp;C3</f>
-        <v>-</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <f t="shared" ref="G3:G4" si="0">+B3&amp;"-"&amp;C3&amp;"-"&amp;D3&amp;"-"&amp;E3&amp;"-"&amp;F3</f>
+        <v>28/04/2024-10:00am-No Reservado-Masaje completo-Chapinero</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="5" t="str">
+      <c r="B4" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>-</v>
+        <v>05/05/2024-12:30pm-Reservado-Chocolaterapia-Bocagrande</v>
       </c>
     </row>
   </sheetData>
@@ -760,119 +934,183 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E27757F1-FD83-4C60-A977-3E4A8F875641}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="E1" sqref="E1:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="5" t="str">
+        <f>+B2&amp;"-"&amp;C2&amp;"-"&amp;D2&amp;"-"&amp;E2&amp;"-"&amp;F2</f>
+        <v>Colombia-Antioquia-Medellín-El poblado-CL 10 43 A 29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G3" s="5" t="str">
+        <f t="shared" ref="G3:G4" si="0">+B3&amp;"-"&amp;C3&amp;"-"&amp;D3&amp;"-"&amp;E3&amp;"-"&amp;F3</f>
+        <v>Colombia-Cundinamarca-Bogotá-Chapinero-CL 63 9 36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="5" t="str">
+        <f t="shared" si="0"/>
+        <v>Colombia-Atlántico-Cartagena-Bocagrande-CR 2 5 39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C51225-C664-4835-BBA4-220D6C13A752}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="5">
-        <f>B2</f>
-        <v>0</v>
+      <c r="B2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="5" t="str">
+        <f>+B2</f>
+        <v>Limpieza facial</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C4" si="0">B3</f>
-        <v>0</v>
+      <c r="B3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <f t="shared" ref="C3:C4" si="0">+B3</f>
+        <v>Masaje completo</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="5">
+      <c r="B4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="5" t="str">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62C51225-C664-4835-BBA4-220D6C13A752}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="5">
-        <f>B2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="5">
-        <f t="shared" ref="C3:C4" si="0">B3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <v>Chocolaterapia</v>
       </c>
     </row>
   </sheetData>

</xml_diff>